<commit_message>
Familiars and Animal Companions now working
Only a few choices fully functional, data entry needed to update skills
to new format
</commit_message>
<xml_diff>
--- a/data/WeaponInfo.xlsx
+++ b/data/WeaponInfo.xlsx
@@ -1152,6 +1152,11 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="1">
+          <cell r="CI1" t="b">
+            <v>0</v>
+          </cell>
+        </row>
         <row r="12">
           <cell r="AA12">
             <v>1</v>
@@ -1261,17 +1266,70 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="I2" t="e">
+            <v>#REF!</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="2">
+          <cell r="I2" t="b">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="2">
+          <cell r="L2">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="3">
+          <cell r="P3" t="e">
+            <v>#NAME?</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7">
+        <row r="1">
+          <cell r="J1" t="str">
+            <v>Abr</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Ability</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="9">
+        <row r="1">
+          <cell r="H1">
+            <v>94</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="10">
+        <row r="1">
+          <cell r="C1" t="e">
+            <v>#N/A</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="11">
+        <row r="5">
+          <cell r="J5" t="str">
+            <v>Fine</v>
+          </cell>
+        </row>
         <row r="9">
           <cell r="B9" t="str">
             <v>Dwarf</v>
@@ -1293,20 +1351,54 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="12"/>
+      <sheetData sheetId="12">
+        <row r="1">
+          <cell r="D1" t="str">
+            <v xml:space="preserve">× Constitution+2, Charisma-2
+× Base land speed of 20 feet.
+× Spell Resistance 
+× Stonecunning: +2 racial bonus on checks to notice unusual stonework. Can find such by passing within 10 feet, and can find stonework traps as a rogue can. Can intuit depth. 
+× Weapon Familiarity: You treat dwarven waraxes and dwarven urgroshes as martial weapons, rather than exotic weapons.
+× Stability: Dwarves are exceptionally stable on their feet. A dwarf gains a +4 bonus on ability checks made to resist being bull rushed or tripped when standing on the ground.
+× +2 racial bonus on saving throws against spells and spell-like effects
+× +1 racial bonus on attack rolls against orcs and goblinoids
+× +4 dodge bonus against creatures of the giant type.
+× +2 racial bonus on Appraise and Craft checks that deal with stone or metal.
+× Favored Class: Fighter
+</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="13">
+        <row r="2">
+          <cell r="AR2" t="str">
+            <v>Swarm Type</v>
+          </cell>
+        </row>
         <row r="4">
           <cell r="AG4" t="str">
             <v/>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
+      <sheetData sheetId="14">
+        <row r="1">
+          <cell r="D1" t="str">
+            <v/>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="15">
+        <row r="2">
+          <cell r="A2">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="16">
         <row r="6">
           <cell r="E6">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="8">
@@ -1336,12 +1428,12 @@
         </row>
         <row r="15">
           <cell r="E15">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="16">
           <cell r="EJ16" t="b">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="17">
@@ -1593,25 +1685,126 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
+      <sheetData sheetId="17">
+        <row r="33">
+          <cell r="H33">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20">
+        <row r="2">
+          <cell r="M2" t="str">
+            <v/>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="21">
+        <row r="5">
+          <cell r="E5" t="str">
+            <v>O</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="22">
+        <row r="1">
+          <cell r="AB1">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="23">
+        <row r="1">
+          <cell r="H1">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="24">
+        <row r="1">
+          <cell r="AK1" t="str">
+            <v>not valid</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="25">
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Soulmeld</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="26">
+        <row r="1">
+          <cell r="G1" t="str">
+            <v/>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="27">
+        <row r="1">
+          <cell r="W1">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="28">
+        <row r="1">
+          <cell r="GR1">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="29">
+        <row r="3">
+          <cell r="G3">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="30">
+        <row r="3">
+          <cell r="O3">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="31">
+        <row r="1">
+          <cell r="G1">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="32">
+        <row r="2">
+          <cell r="E2">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="33">
+        <row r="3">
+          <cell r="E3">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="34">
+        <row r="1">
+          <cell r="Y1" t="b">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="35">
+        <row r="1">
+          <cell r="F1">
+            <v>1</v>
+          </cell>
+        </row>
         <row r="54">
           <cell r="AR54" t="b">
             <v>0</v>
@@ -1730,6 +1923,9 @@
       </sheetData>
       <sheetData sheetId="36">
         <row r="1">
+          <cell r="H1" t="str">
+            <v>(none)</v>
+          </cell>
           <cell r="Q1">
             <v>0</v>
           </cell>
@@ -1740,33 +1936,139 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
+      <sheetData sheetId="37">
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>Select A Weapon</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="38">
+        <row r="2">
+          <cell r="C2">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="39">
+        <row r="2">
+          <cell r="J2" t="str">
+            <v>(none)</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="40">
+        <row r="2">
+          <cell r="W2" t="b">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="41">
+        <row r="19">
+          <cell r="CJ19" t="str">
+            <v/>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="42">
+        <row r="63">
+          <cell r="BA63">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44">
+        <row r="3">
+          <cell r="CZ3" t="str">
+            <v>strmod</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47">
+        <row r="3">
+          <cell r="DB3" t="e">
+            <v>#N/A</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="48">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v/>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="49">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v/>
+          </cell>
+        </row>
         <row r="4538">
           <cell r="E4538">
             <v>0</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
+      <sheetData sheetId="50">
+        <row r="1">
+          <cell r="U1" t="str">
+            <v>Arms</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="51">
+        <row r="5">
+          <cell r="C5" t="str">
+            <v/>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="52">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Select A Deity</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="53">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Air</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="54">
+        <row r="3">
+          <cell r="N3" t="str">
+            <v>Select Spell Casting Class</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="55">
+        <row r="3">
+          <cell r="A3">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="56">
+        <row r="3">
+          <cell r="A3">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="57">
+        <row r="3">
+          <cell r="L3" t="str">
+            <v>Select Manifesting Class</v>
+          </cell>
+        </row>
         <row r="4">
           <cell r="A4" t="str">
             <v>Ardent</v>
@@ -2056,13 +2358,24 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
+      <sheetData sheetId="58" refreshError="1"/>
+      <sheetData sheetId="59" refreshError="1"/>
+      <sheetData sheetId="60" refreshError="1"/>
+      <sheetData sheetId="61">
+        <row r="1">
+          <cell r="A1">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="62" refreshError="1"/>
+      <sheetData sheetId="63" refreshError="1"/>
       <sheetData sheetId="64">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Saving Throw</v>
+          </cell>
+        </row>
         <row r="33">
           <cell r="B33" t="str">
             <v/>
@@ -3027,10 +3340,10 @@
   <dimension ref="A1:P257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P18" sqref="P18"/>
+      <selection pane="bottomRight" activeCell="O138" sqref="O138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4350,7 +4663,7 @@
       </c>
       <c r="P43" t="b">
         <f>OR(DrdLvl&gt;=1,MnkLvl&gt;=1,WizLvl&gt;=1,SmnLvl&gt;=1,PsiLvl&gt;=1,YWRLvl&gt;=1,AND(INDEX(TblSimpleList,CommonerProf)=A43,ComLvl&gt;=1),AND(NoShLvl&gt;=1,OR(NomadShamanRegionCell=3,NomadShamanRegionCell=4,NomadShamanRegionCell=6)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -4537,7 +4850,7 @@
       </c>
       <c r="P49" t="b">
         <f>OR(MnkLvl&gt;=1,WizLvl&gt;=1,AsnLvl&gt;=1,PsiLvl&gt;=1,YWRLvl&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -7247,7 +7560,7 @@
       </c>
       <c r="P138" t="b">
         <f>OR(AND(Race="Elf",Subrace&lt;&gt;"Drow",Subrace&lt;&gt;"Aquatic",Subrace&lt;&gt;"Wild",Subrace&lt;&gt;"Kagonesti",Subrace&lt;&gt;"Forestlord"),FullRace="Centaur",BrdLvl&gt;=1,FMkLvl&gt;=1,FullRace="Draconian, Baaz",AND(RuaLvl&gt;=1,RuatharMartialWeaponCell=2),MnfLvl&gt;=1,DrPgLvl&gt;0,AND(BinLvl&gt;=1,NOT(ISERROR(MATCH("Andras",VestigesSelected,0)))),AND(BinLvl&gt;=1,NOT(ISERROR(MATCH("Kas",VestigesSelected,0)))))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
@@ -8221,7 +8534,7 @@
       </c>
       <c r="P171" t="b">
         <f>OR(DrdLvl&gt;=1,MnkLvl&gt;=1,WizLvl&gt;=1,SmnLvl&gt;=1,PsiLvl&gt;=1,YWRLvl&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.25">
@@ -10586,7 +10899,7 @@
       </c>
       <c r="P249" t="b">
         <f>OR(BrdLvl&gt;=1,HthLvl&gt;=1,FMkLvl&gt;=1,MoPLvl&gt;=1,AND(NoShLvl&gt;=1,OR(NomadShamanRegionCell=2,NomadShamanRegionCell=6)),AND(CrSLvl&gt;=1,CrSWeaponProf=4))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:16" x14ac:dyDescent="0.25">
@@ -10680,7 +10993,7 @@
       </c>
       <c r="P252" t="b">
         <f>BrdLvl&gt;=1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>